<commit_message>
added updated colab and excel
</commit_message>
<xml_diff>
--- a/analysis_and_resources/model_optimization.xlsx
+++ b/analysis_and_resources/model_optimization.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4411de4da39a5aa/Desktop/VandyDataCourse/project_4/Starter_Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4411de4da39a5aa/Desktop/VandyDataCourse/project_4/analysis_and_resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD24B7C3-1458-4B90-ABFC-F5E47F242FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{A4E3FF4F-D51E-42F3-BFB3-CD3B024C260A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="-16125" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{17C16DA7-B2F8-49D5-A81C-A95D4F5BD202}"/>
+    <workbookView xWindow="9450" yWindow="-15480" windowWidth="17265" windowHeight="8880" xr2:uid="{17C16DA7-B2F8-49D5-A81C-A95D4F5BD202}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomForest" sheetId="1" r:id="rId1"/>
-    <sheet name="NeuralNetwork" sheetId="3" r:id="rId2"/>
+    <sheet name="RandomForestWOutlierControl" sheetId="4" r:id="rId2"/>
+    <sheet name="NeuralNetwork" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Parameters</t>
   </si>
@@ -112,12 +113,30 @@
   <si>
     <t xml:space="preserve">Nodes (not including output layer) </t>
   </si>
+  <si>
+    <t>relu/linear</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>layer 4</t>
+  </si>
+  <si>
+    <t>Max Depth </t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,40 +170,55 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13.95"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13.95"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAB40"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -192,172 +226,61 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF5E5E5E"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF5E5E5E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF5E5E5E"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF5E5E5E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF5E5E5E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF5E5E5E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF5E5E5E"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF5E5E5E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF5E5E5E"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF5E5E5E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF5E5E5E"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF5E5E5E"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF5E5E5E"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF5E5E5E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF5E5E5E"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF5E5E5E"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF5E5E5E"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF5E5E5E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF5E5E5E"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF5E5E5E"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF5E5E5E"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,6 +296,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -694,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA97CCF4-93BD-4FED-8CC0-889213BDCCDE}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,134 +632,134 @@
     <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="13">
         <v>100</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="13">
         <v>364.57</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="13">
         <v>0.95</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="13">
         <v>0.98</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
         <v>10</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="13">
         <v>100</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="13">
         <v>326.99</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="13">
         <v>1.91</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="13">
         <v>0.98</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
         <v>60</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="13">
         <v>200</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="13">
         <v>336.49</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="13">
         <v>0.94</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="13">
         <v>0.98</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
         <v>100</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="13">
         <v>600</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="13">
         <v>297.05</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="13">
         <v>0.92</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="13">
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
         <v>200</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="13">
         <v>1500</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="13">
         <v>327.18</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="13">
         <v>0.94</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="13">
         <v>0.98</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="13">
         <v>3000</v>
       </c>
-      <c r="C8" s="7">
-        <v>11938.9</v>
-      </c>
-      <c r="D8" s="4">
-        <v>16.82</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.4</v>
+      <c r="C8" s="15">
+        <v>314.83</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.94</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>
@@ -845,11 +772,168 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4587B0B-29D2-4F89-B98D-B54BA7AFCB2D}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10803.24</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9.94</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>250</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10803.05</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9.94</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>800</v>
+      </c>
+      <c r="C5" s="4">
+        <v>10802.79</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9.94</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>100</v>
+      </c>
+      <c r="C6" s="4">
+        <v>10803.78</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10.24</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>250</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10803.05</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.94</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>500</v>
+      </c>
+      <c r="B8" s="2">
+        <v>800</v>
+      </c>
+      <c r="C8" s="4">
+        <v>10802.79</v>
+      </c>
+      <c r="D8" s="2">
+        <v>9.94</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2127A8FC-C21D-49EC-B65D-822EC109D231}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,174 +945,287 @@
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="17"/>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
+      <c r="I2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="F3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="12">
-        <v>6</v>
-      </c>
-      <c r="D4" s="12">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="2">
+        <v>6</v>
+      </c>
+      <c r="D4" s="11">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="12">
+      <c r="G4" s="2">
         <v>50</v>
       </c>
-      <c r="G4" s="12">
+      <c r="H4" s="2">
         <v>32.17</v>
       </c>
-      <c r="H4" s="12">
+      <c r="I4" s="2">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="2">
         <v>8</v>
       </c>
-      <c r="D5" s="12">
-        <v>6</v>
-      </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="11">
+        <v>6</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="12">
+      <c r="G5" s="2">
         <v>50</v>
       </c>
-      <c r="G5" s="12">
+      <c r="H5" s="2">
         <v>33.47</v>
       </c>
-      <c r="H5" s="12">
+      <c r="I5" s="2">
         <v>2.66</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6</v>
+      </c>
+      <c r="D6" s="11">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2">
+        <v>100</v>
+      </c>
+      <c r="H6" s="2">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2.08</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11">
+        <v>6</v>
+      </c>
+      <c r="E7" s="11">
+        <v>6</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2">
+        <v>82.83</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
         <v>8</v>
       </c>
-      <c r="D6" s="12">
-        <v>6</v>
-      </c>
-      <c r="E6" s="12">
-        <v>6</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="D8" s="11">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11">
+        <v>6</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2">
         <v>50</v>
       </c>
-      <c r="G6" s="12">
-        <v>22.2</v>
-      </c>
-      <c r="H6" s="12">
-        <v>2.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+      <c r="H8" s="2">
+        <v>27.36</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B9" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C9" s="2">
         <v>8</v>
       </c>
-      <c r="D7" s="12">
-        <v>6</v>
-      </c>
-      <c r="E7" s="12">
-        <v>6</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="D9" s="11">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2">
+        <v>50</v>
+      </c>
+      <c r="H9" s="2">
+        <v>58.26</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2.75</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="D10" s="11">
+        <v>6</v>
+      </c>
+      <c r="E10" s="11">
+        <v>6</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2">
         <v>100</v>
       </c>
-      <c r="G7" s="12">
+      <c r="H10" s="2">
         <v>63.91</v>
       </c>
-      <c r="H7" s="12">
+      <c r="I10" s="2">
         <v>5.16</v>
       </c>
+      <c r="J10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:F2"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I2:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>